<commit_message>
Filtros de parametros para generar la hoja de calculo
</commit_message>
<xml_diff>
--- a/Payroll/Content/REPORTES/NOMINA/HCalculo_E2_A2020_NP23_TP3_A.xlsx
+++ b/Payroll/Content/REPORTES/NOMINA/HCalculo_E2_A2020_NP23_TP3_A.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>AÑO</t>
   </si>
@@ -110,34 +110,10 @@
     <t>(32)Dias Cotizados</t>
   </si>
   <si>
-    <t>(1)Sueldo</t>
-  </si>
-  <si>
-    <t>(5)Premio de Asistencia</t>
-  </si>
-  <si>
-    <t>(6)Premio de Puntualidad</t>
-  </si>
-  <si>
-    <t>(17)Despensa en Efectivo</t>
-  </si>
-  <si>
     <t>(126)Pago Beca</t>
   </si>
   <si>
     <t>(990)Total de Percepciones</t>
-  </si>
-  <si>
-    <t>(1001)ISR</t>
-  </si>
-  <si>
-    <t>(1013)Falta Injustificada</t>
-  </si>
-  <si>
-    <t>(1310)Cuota IMSS Empleado</t>
-  </si>
-  <si>
-    <t>(1311)Dscto Retiro por Cesantia y Vejez</t>
   </si>
   <si>
     <t>(1990)Total de Deducciones</t>
@@ -344,7 +320,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:AW5"/>
+  <dimension ref="A1:AO5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -453,47 +429,23 @@
       <c r="AI1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AK1" s="4" t="s">
         <v>35</v>
       </c>
       <c r="AL1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AO1" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="AN1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AO1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AP1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AQ1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AR1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AS1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AU1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AV1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AW1" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2">
@@ -507,73 +459,73 @@
         <v>2</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E2" s="6">
         <v>501829</v>
       </c>
       <c r="F2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="O2" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" s="0" t="s">
+      <c r="P2" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q2" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>58</v>
-      </c>
       <c r="R2" s="0" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="S2" s="6">
         <v>1</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="V2" s="6">
         <v>1</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="Z2" s="0" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="AA2" s="7">
         <v>125000</v>
@@ -593,52 +545,28 @@
       <c r="AG2" s="7">
         <v>15</v>
       </c>
-      <c r="AH2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI2" s="0" t="s">
-        <v>61</v>
+      <c r="AH2" s="7">
+        <v>62500</v>
+      </c>
+      <c r="AI2" s="7">
+        <v>62500</v>
       </c>
       <c r="AJ2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AK2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AL2" s="7">
+        <v>53</v>
+      </c>
+      <c r="AK2" s="8">
         <v>62500</v>
       </c>
-      <c r="AM2" s="7">
-        <v>62500</v>
-      </c>
-      <c r="AN2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AO2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AP2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AQ2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AR2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AS2" s="8">
-        <v>62500</v>
-      </c>
-      <c r="AT2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AU2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AV2" s="9">
+      <c r="AL2" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM2" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN2" s="9">
         <v>0</v>
       </c>
-      <c r="AW2" s="10">
+      <c r="AO2" s="10">
         <v>62500</v>
       </c>
     </row>
@@ -653,73 +581,73 @@
         <v>2</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E3" s="6">
         <v>902758</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="S3" s="6">
         <v>1</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="V3" s="6">
         <v>1</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="Y3" s="0" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="Z3" s="0" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="AA3" s="7">
         <v>4000</v>
@@ -739,52 +667,28 @@
       <c r="AG3" s="7">
         <v>15</v>
       </c>
-      <c r="AH3" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI3" s="0" t="s">
-        <v>61</v>
+      <c r="AH3" s="7">
+        <v>2000</v>
+      </c>
+      <c r="AI3" s="7">
+        <v>2000</v>
       </c>
       <c r="AJ3" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AK3" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AL3" s="7">
+        <v>53</v>
+      </c>
+      <c r="AK3" s="8">
         <v>2000</v>
       </c>
-      <c r="AM3" s="7">
-        <v>2000</v>
-      </c>
-      <c r="AN3" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AO3" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AP3" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AQ3" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AR3" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AS3" s="8">
-        <v>2000</v>
-      </c>
-      <c r="AT3" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AU3" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AV3" s="9">
+      <c r="AL3" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM3" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN3" s="9">
         <v>0</v>
       </c>
-      <c r="AW3" s="10">
+      <c r="AO3" s="10">
         <v>2000</v>
       </c>
     </row>
@@ -799,73 +703,73 @@
         <v>2</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E4" s="6">
         <v>903645</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="S4" s="6">
         <v>1</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="U4" s="0" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="V4" s="6">
         <v>1</v>
       </c>
       <c r="W4" s="0" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="X4" s="0" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="Y4" s="0" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="Z4" s="0" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="AA4" s="7">
         <v>5500</v>
@@ -885,52 +789,28 @@
       <c r="AG4" s="7">
         <v>14</v>
       </c>
-      <c r="AH4" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI4" s="0" t="s">
-        <v>61</v>
+      <c r="AH4" s="7">
+        <v>2566.67</v>
+      </c>
+      <c r="AI4" s="7">
+        <v>2566.67</v>
       </c>
       <c r="AJ4" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AK4" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AL4" s="7">
+        <v>53</v>
+      </c>
+      <c r="AK4" s="8">
         <v>2566.67</v>
       </c>
-      <c r="AM4" s="7">
-        <v>2566.67</v>
-      </c>
-      <c r="AN4" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AO4" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AP4" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AQ4" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AR4" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AS4" s="8">
-        <v>2566.67</v>
-      </c>
-      <c r="AT4" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AU4" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AV4" s="9">
+      <c r="AL4" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM4" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN4" s="9">
         <v>0</v>
       </c>
-      <c r="AW4" s="10">
+      <c r="AO4" s="10">
         <v>2566.67</v>
       </c>
     </row>
@@ -945,73 +825,73 @@
         <v>2</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E5" s="6">
         <v>903646</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="S5" s="6">
         <v>1</v>
       </c>
       <c r="T5" s="0" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="U5" s="0" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="V5" s="6">
         <v>1</v>
       </c>
       <c r="W5" s="0" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="X5" s="0" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="Y5" s="0" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="Z5" s="0" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="AA5" s="7">
         <v>5500</v>
@@ -1031,52 +911,28 @@
       <c r="AG5" s="7">
         <v>14</v>
       </c>
-      <c r="AH5" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI5" s="0" t="s">
-        <v>61</v>
+      <c r="AH5" s="7">
+        <v>2566.67</v>
+      </c>
+      <c r="AI5" s="7">
+        <v>2566.67</v>
       </c>
       <c r="AJ5" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AK5" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AL5" s="7">
+        <v>53</v>
+      </c>
+      <c r="AK5" s="8">
         <v>2566.67</v>
       </c>
-      <c r="AM5" s="7">
-        <v>2566.67</v>
-      </c>
-      <c r="AN5" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AO5" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AP5" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AQ5" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AR5" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AS5" s="8">
-        <v>2566.67</v>
-      </c>
-      <c r="AT5" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AU5" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AV5" s="9">
+      <c r="AL5" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM5" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN5" s="9">
         <v>0</v>
       </c>
-      <c r="AW5" s="10">
+      <c r="AO5" s="10">
         <v>2566.67</v>
       </c>
     </row>

</xml_diff>